<commit_message>
Feat: new batch data and optimization tests
</commit_message>
<xml_diff>
--- a/dados/Semibat_convertido_clean.xlsx
+++ b/dados/Semibat_convertido_clean.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\Desktop\lneoc\pibic_lneoc\SINDy\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\Desktop\lneoc\estágio_viegas\Gepam\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B52FFA5E-AFEB-467C-95EB-455B9B469D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07D7185-96BE-4C38-AFDE-C78B939996FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F6C2ECE7-9ED1-4A12-BCC5-5F1DAF65C722}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="10968" windowHeight="12336" xr2:uid="{F6C2ECE7-9ED1-4A12-BCC5-5F1DAF65C722}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -432,7 +432,7 @@
   <dimension ref="A1:AI32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22:K24"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,11 +490,11 @@
         <v>15.070093457943925</v>
       </c>
       <c r="K2" s="2">
-        <v>-2.4539877300613498E-2</v>
+        <v>0</v>
       </c>
       <c r="L2" s="3">
         <f>(K2/167.16)*1000</f>
-        <v>-0.14680472182707285</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.3">

</xml_diff>